<commit_message>
Update product backlog. Remove sprint 6. Update Userguide
</commit_message>
<xml_diff>
--- a/Document/Product Backlog-en.xlsx
+++ b/Document/Product Backlog-en.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
   <si>
     <t>Sprint</t>
   </si>
@@ -201,9 +201,6 @@
     <t>Display order's history of customers</t>
   </si>
   <si>
-    <t>Menu</t>
-  </si>
-  <si>
     <t>Provide a private account for restaurant manager</t>
   </si>
   <si>
@@ -213,15 +210,6 @@
     <t>Customer</t>
   </si>
   <si>
-    <t>Show menu of the selected restaurant</t>
-  </si>
-  <si>
-    <t>Display all infomations about all dishes in the menu</t>
-  </si>
-  <si>
-    <t>Display statuses of all dishes which include attribute new</t>
-  </si>
-  <si>
     <t>Be able to modify customer information</t>
   </si>
   <si>
@@ -229,6 +217,9 @@
   </si>
   <si>
     <t>Customer information</t>
+  </si>
+  <si>
+    <t>dong</t>
   </si>
 </sst>
 </file>
@@ -271,7 +262,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -305,18 +296,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCFE2F3"/>
-        <bgColor rgb="FFCFE2F3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor rgb="FFCFE2F3"/>
       </patternFill>
     </fill>
@@ -495,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -584,54 +563,56 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -658,43 +639,23 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -976,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z995"/>
+  <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1042,10 +1003,10 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45">
+      <c r="A2" s="48">
         <v>1</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="50" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1086,12 +1047,12 @@
       <c r="Z2" s="3"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="46"/>
+      <c r="A3" s="49"/>
       <c r="B3" s="40"/>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="50" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="5" t="s">
@@ -1105,7 +1066,7 @@
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="5" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -1126,10 +1087,10 @@
       <c r="Z3" s="3"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="46"/>
+      <c r="A4" s="49"/>
       <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
       <c r="E4" s="5" t="s">
         <v>19</v>
       </c>
@@ -1141,7 +1102,7 @@
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -1162,8 +1123,8 @@
       <c r="Z4" s="3"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="47"/>
-      <c r="B5" s="41"/>
+      <c r="A5" s="38"/>
+      <c r="B5" s="42"/>
       <c r="C5" s="6" t="s">
         <v>10</v>
       </c>
@@ -1202,10 +1163,10 @@
       <c r="Z5" s="3"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="50">
+      <c r="A6" s="52">
         <v>2</v>
       </c>
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="55" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="17" t="s">
@@ -1244,16 +1205,16 @@
       <c r="Z6" s="3"/>
     </row>
     <row r="7" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="51"/>
-      <c r="B7" s="54"/>
-      <c r="C7" s="49" t="s">
+      <c r="A7" s="53"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="51" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>29</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F7" s="22">
         <v>1</v>
@@ -1282,9 +1243,9 @@
       <c r="Z7" s="3"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="52"/>
-      <c r="B8" s="55"/>
-      <c r="C8" s="41"/>
+      <c r="A8" s="54"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="42"/>
       <c r="D8" s="7" t="s">
         <v>30</v>
       </c>
@@ -1320,10 +1281,10 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="56">
+      <c r="A9" s="37">
         <v>3</v>
       </c>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="41" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="9" t="s">
@@ -1362,8 +1323,8 @@
       <c r="Z9" s="3"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="47"/>
-      <c r="B10" s="41"/>
+      <c r="A10" s="38"/>
+      <c r="B10" s="42"/>
       <c r="C10" s="9" t="s">
         <v>35</v>
       </c>
@@ -1371,7 +1332,7 @@
         <v>36</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F10" s="23">
         <v>1</v>
@@ -1381,7 +1342,7 @@
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -1402,7 +1363,7 @@
       <c r="Z10" s="3"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="59">
+      <c r="A11" s="46">
         <v>4</v>
       </c>
       <c r="B11" s="39" t="s">
@@ -1417,7 +1378,7 @@
       <c r="E11" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="42">
+      <c r="F11" s="58">
         <v>1</v>
       </c>
       <c r="G11" s="39" t="s">
@@ -1446,14 +1407,14 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="1:26" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="57"/>
+      <c r="A12" s="47"/>
       <c r="B12" s="40"/>
       <c r="C12" s="40"/>
       <c r="D12" s="40"/>
       <c r="E12" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="43"/>
+      <c r="F12" s="59"/>
       <c r="G12" s="40"/>
       <c r="H12" s="40"/>
       <c r="I12" s="11" t="s">
@@ -1478,18 +1439,18 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="1:26" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="57"/>
+      <c r="A13" s="47"/>
       <c r="B13" s="40"/>
       <c r="C13" s="40"/>
-      <c r="D13" s="41"/>
+      <c r="D13" s="42"/>
       <c r="E13" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="44"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
       <c r="I13" s="14" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -1510,7 +1471,7 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A14" s="57"/>
+      <c r="A14" s="47"/>
       <c r="B14" s="40"/>
       <c r="C14" s="40"/>
       <c r="D14" s="39" t="s">
@@ -1519,7 +1480,7 @@
       <c r="E14" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="42">
+      <c r="F14" s="58">
         <v>1</v>
       </c>
       <c r="G14" s="39" t="s">
@@ -1548,14 +1509,14 @@
       <c r="Z14" s="3"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A15" s="57"/>
+      <c r="A15" s="47"/>
       <c r="B15" s="40"/>
       <c r="C15" s="40"/>
       <c r="D15" s="40"/>
       <c r="E15" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="43"/>
+      <c r="F15" s="59"/>
       <c r="G15" s="40"/>
       <c r="H15" s="40"/>
       <c r="I15" s="40"/>
@@ -1578,14 +1539,14 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A16" s="57"/>
+      <c r="A16" s="47"/>
       <c r="B16" s="40"/>
       <c r="C16" s="40"/>
       <c r="D16" s="40"/>
       <c r="E16" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="F16" s="43"/>
+      <c r="F16" s="59"/>
       <c r="G16" s="40"/>
       <c r="H16" s="40"/>
       <c r="I16" s="40"/>
@@ -1608,17 +1569,17 @@
       <c r="Z16" s="3"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A17" s="57"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="40"/>
       <c r="C17" s="40"/>
       <c r="D17" s="40"/>
       <c r="E17" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="44"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
@@ -1638,10 +1599,10 @@
       <c r="Z17" s="3"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A18" s="57"/>
+      <c r="A18" s="47"/>
       <c r="B18" s="40"/>
       <c r="C18" s="40"/>
-      <c r="D18" s="41"/>
+      <c r="D18" s="42"/>
       <c r="E18" s="14" t="s">
         <v>50</v>
       </c>
@@ -1674,25 +1635,25 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A19" s="69">
+      <c r="A19" s="43">
         <v>5</v>
       </c>
       <c r="B19" s="40"/>
       <c r="C19" s="40"/>
-      <c r="D19" s="62" t="s">
+      <c r="D19" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="63" t="s">
+      <c r="E19" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="F19" s="64">
+      <c r="F19" s="31">
         <v>2</v>
       </c>
-      <c r="G19" s="63" t="s">
+      <c r="G19" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="63"/>
-      <c r="I19" s="63" t="s">
+      <c r="H19" s="30"/>
+      <c r="I19" s="30" t="s">
         <v>27</v>
       </c>
       <c r="J19" s="3"/>
@@ -1714,19 +1675,19 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A20" s="60"/>
+      <c r="A20" s="44"/>
       <c r="B20" s="40"/>
       <c r="C20" s="40"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="63" t="s">
+      <c r="D20" s="35"/>
+      <c r="E20" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="F20" s="64">
+      <c r="F20" s="31">
         <v>3</v>
       </c>
-      <c r="G20" s="63"/>
-      <c r="H20" s="63"/>
-      <c r="I20" s="63" t="s">
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30" t="s">
         <v>27</v>
       </c>
       <c r="J20" s="3"/>
@@ -1748,21 +1709,21 @@
       <c r="Z20" s="3"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A21" s="60"/>
+      <c r="A21" s="44"/>
       <c r="B21" s="40"/>
       <c r="C21" s="40"/>
-      <c r="D21" s="66"/>
-      <c r="E21" s="63" t="s">
+      <c r="D21" s="36"/>
+      <c r="E21" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="64">
+      <c r="F21" s="31">
         <v>3</v>
       </c>
-      <c r="G21" s="63" t="s">
+      <c r="G21" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="63"/>
-      <c r="I21" s="63" t="s">
+      <c r="H21" s="30"/>
+      <c r="I21" s="30" t="s">
         <v>27</v>
       </c>
       <c r="J21" s="3"/>
@@ -1784,19 +1745,19 @@
       <c r="Z21" s="3"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A22" s="61"/>
+      <c r="A22" s="45"/>
       <c r="B22" s="40"/>
       <c r="C22" s="40"/>
-      <c r="D22" s="67" t="s">
+      <c r="D22" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="67"/>
-      <c r="F22" s="68">
+      <c r="E22" s="32"/>
+      <c r="F22" s="33">
         <v>4</v>
       </c>
-      <c r="G22" s="67"/>
-      <c r="H22" s="67"/>
-      <c r="I22" s="67" t="s">
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32" t="s">
         <v>27</v>
       </c>
       <c r="J22" s="3"/>
@@ -1817,30 +1778,28 @@
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
     </row>
-    <row r="23" spans="1:26" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="37">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A23" s="61">
         <v>6</v>
       </c>
-      <c r="B23" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="E23" s="27" t="s">
+      <c r="B23" s="62" t="s">
         <v>61</v>
       </c>
+      <c r="C23" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="63"/>
+      <c r="E23" s="27" t="s">
+        <v>59</v>
+      </c>
       <c r="F23" s="28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G23" s="27" t="s">
         <v>13</v>
       </c>
       <c r="H23" s="29"/>
-      <c r="I23" s="30" t="s">
+      <c r="I23" s="29" t="s">
         <v>27</v>
       </c>
       <c r="J23" s="3"/>
@@ -1861,22 +1820,22 @@
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
     </row>
-    <row r="24" spans="1:26" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="37"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A24" s="61"/>
+      <c r="B24" s="62"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="63"/>
       <c r="E24" s="27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F24" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G24" s="27" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="H24" s="29"/>
-      <c r="I24" s="30" t="s">
+      <c r="I24" s="29" t="s">
         <v>27</v>
       </c>
       <c r="J24" s="3"/>
@@ -1898,27 +1857,15 @@
       <c r="Z24" s="3"/>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A25" s="34">
-        <v>7</v>
-      </c>
-      <c r="B25" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="D25" s="36"/>
-      <c r="E25" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="F25" s="32">
-        <v>2</v>
-      </c>
-      <c r="G25" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
@@ -1938,21 +1885,15 @@
       <c r="Z25" s="3"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A26" s="34"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="F26" s="32">
-        <v>1</v>
-      </c>
-      <c r="G26" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
@@ -29047,64 +28988,26 @@
       <c r="Y993" s="3"/>
       <c r="Z993" s="3"/>
     </row>
-    <row r="994" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A994" s="15"/>
-      <c r="B994" s="3"/>
-      <c r="C994" s="3"/>
-      <c r="D994" s="3"/>
-      <c r="E994" s="3"/>
-      <c r="F994" s="25"/>
-      <c r="G994" s="3"/>
-      <c r="H994" s="3"/>
-      <c r="I994" s="3"/>
-      <c r="J994" s="3"/>
-      <c r="K994" s="3"/>
-      <c r="L994" s="3"/>
-      <c r="M994" s="3"/>
-      <c r="N994" s="3"/>
-      <c r="O994" s="3"/>
-      <c r="P994" s="3"/>
-      <c r="Q994" s="3"/>
-      <c r="R994" s="3"/>
-      <c r="S994" s="3"/>
-      <c r="T994" s="3"/>
-      <c r="U994" s="3"/>
-      <c r="V994" s="3"/>
-      <c r="W994" s="3"/>
-      <c r="X994" s="3"/>
-      <c r="Y994" s="3"/>
-      <c r="Z994" s="3"/>
-    </row>
-    <row r="995" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A995" s="15"/>
-      <c r="B995" s="3"/>
-      <c r="C995" s="3"/>
-      <c r="D995" s="3"/>
-      <c r="E995" s="3"/>
-      <c r="F995" s="25"/>
-      <c r="G995" s="3"/>
-      <c r="H995" s="3"/>
-      <c r="I995" s="3"/>
-      <c r="J995" s="3"/>
-      <c r="K995" s="3"/>
-      <c r="L995" s="3"/>
-      <c r="M995" s="3"/>
-      <c r="N995" s="3"/>
-      <c r="O995" s="3"/>
-      <c r="P995" s="3"/>
-      <c r="Q995" s="3"/>
-      <c r="R995" s="3"/>
-      <c r="S995" s="3"/>
-      <c r="T995" s="3"/>
-      <c r="U995" s="3"/>
-      <c r="V995" s="3"/>
-      <c r="W995" s="3"/>
-      <c r="X995" s="3"/>
-      <c r="Y995" s="3"/>
-      <c r="Z995" s="3"/>
-    </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="27">
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="G14:G17"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="I14:I17"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
     <mergeCell ref="D19:D21"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B11:B22"/>
@@ -29114,28 +29017,6 @@
     <mergeCell ref="D11:D13"/>
     <mergeCell ref="A19:A22"/>
     <mergeCell ref="A11:A18"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="G14:G17"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="I14:I17"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="H11:H13"/>
-    <mergeCell ref="F14:F17"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>